<commit_message>
verify data integrity and add flesh out visualizations
</commit_message>
<xml_diff>
--- a/data/raw/CDS_25_Task2.xlsx
+++ b/data/raw/CDS_25_Task2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\DS Projects\NLP_Call_Script_Analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\DS Projects\NLP_Call_Script_Analysis\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660132D7-9AA3-46B1-8C0F-32EF57A46C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE404ED3-3B59-4432-9486-1D52B9E5E46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5C99187-B74D-41F0-823D-0C9369D594C0}"/>
   </bookViews>
@@ -15129,8 +15129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA6D646-C9D9-4E25-B10C-8DA8BDC22043}">
   <dimension ref="A1:M381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F346" workbookViewId="0">
-      <selection activeCell="F372" sqref="F372"/>
+    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="E217" sqref="E217:E285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15139,7 +15139,7 @@
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="162.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="228.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="149" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>